<commit_message>
Added minor Nubri varieties and  tidied conversion code for various languages
</commit_message>
<xml_diff>
--- a/data/processed/progress.xlsx
+++ b/data/processed/progress.xlsx
@@ -1,96 +1,112 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26505"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sgroberts/Documents/Funding/InternationalStrategicFund/project/data/processed/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="17820" windowHeight="9420"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
-  <si>
-    <t>language</t>
-  </si>
-  <si>
-    <t>numEntries</t>
-  </si>
-  <si>
-    <t>numConceptsMatchedToConcepticon</t>
-  </si>
-  <si>
-    <t>numSwadesh100ConceptsMatchedToConcepticon</t>
-  </si>
-  <si>
-    <t>numJirel208ConceptsMatchedToConcepticon</t>
-  </si>
-  <si>
-    <t>progress</t>
-  </si>
-  <si>
-    <t>tsum</t>
-  </si>
-  <si>
-    <t>82%</t>
-  </si>
-  <si>
-    <t>nubri</t>
-  </si>
-  <si>
-    <t>60%</t>
-  </si>
-  <si>
-    <t>gyalsumdo</t>
-  </si>
-  <si>
-    <t>64%</t>
-  </si>
-  <si>
-    <t>jirel</t>
-  </si>
-  <si>
-    <t>100%</t>
-  </si>
-  <si>
-    <t>lowa</t>
-  </si>
-  <si>
-    <t>43%</t>
-  </si>
-  <si>
-    <t>yolmo</t>
-  </si>
-  <si>
-    <t>62%</t>
-  </si>
-  <si>
-    <t>kagate</t>
-  </si>
-  <si>
-    <t>79%</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+  <si>
+    <t xml:space="preserve">language</t>
+  </si>
+  <si>
+    <t xml:space="preserve">numEntries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">numConceptsMatchedToConcepticon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">numSwadesh100ConceptsMatchedToConcepticon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">numJirel208ConceptsMatchedToConcepticon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">progress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tsum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">82%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nubri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nubri_namrung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">95%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nubri_lhi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">94%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nubri_lho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nubri_sama</t>
+  </si>
+  <si>
+    <t xml:space="preserve">88%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nubri_sho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">93%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gyalsumdo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">64%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jirel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lowa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">43%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yolmo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">62%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kagate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">79%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -126,12 +142,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -413,24 +423,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.5" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -450,148 +450,248 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="n">
         <v>2445</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="n">
         <v>854</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="n">
         <v>81</v>
       </c>
-      <c r="E2">
+      <c r="E2" t="n">
         <v>171</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="n">
         <v>2170</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="n">
         <v>601</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="n">
         <v>60</v>
       </c>
-      <c r="E3">
+      <c r="E3" t="n">
         <v>125</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4">
-        <v>2315</v>
-      </c>
-      <c r="C4">
-        <v>671</v>
-      </c>
-      <c r="D4">
-        <v>70</v>
-      </c>
-      <c r="E4">
-        <v>134</v>
+      <c r="B4" t="n">
+        <v>199</v>
+      </c>
+      <c r="C4" t="n">
+        <v>198</v>
+      </c>
+      <c r="D4" t="n">
+        <v>68</v>
+      </c>
+      <c r="E4" t="n">
+        <v>197</v>
       </c>
       <c r="F4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5">
       <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5">
-        <v>210</v>
-      </c>
-      <c r="C5">
-        <v>208</v>
-      </c>
-      <c r="D5">
-        <v>68</v>
-      </c>
-      <c r="E5">
-        <v>208</v>
+      <c r="B5" t="n">
+        <v>198</v>
+      </c>
+      <c r="C5" t="n">
+        <v>197</v>
+      </c>
+      <c r="D5" t="n">
+        <v>67</v>
+      </c>
+      <c r="E5" t="n">
+        <v>196</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6">
       <c r="A6" t="s">
         <v>14</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="n">
+        <v>199</v>
+      </c>
+      <c r="C6" t="n">
+        <v>198</v>
+      </c>
+      <c r="D6" t="n">
+        <v>67</v>
+      </c>
+      <c r="E6" t="n">
+        <v>197</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="n">
+        <v>185</v>
+      </c>
+      <c r="C7" t="n">
+        <v>185</v>
+      </c>
+      <c r="D7" t="n">
+        <v>66</v>
+      </c>
+      <c r="E7" t="n">
+        <v>184</v>
+      </c>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="n">
+        <v>195</v>
+      </c>
+      <c r="C8" t="n">
+        <v>194</v>
+      </c>
+      <c r="D8" t="n">
+        <v>67</v>
+      </c>
+      <c r="E8" t="n">
+        <v>193</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="n">
+        <v>2315</v>
+      </c>
+      <c r="C9" t="n">
+        <v>671</v>
+      </c>
+      <c r="D9" t="n">
+        <v>70</v>
+      </c>
+      <c r="E9" t="n">
+        <v>134</v>
+      </c>
+      <c r="F9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="n">
+        <v>210</v>
+      </c>
+      <c r="C10" t="n">
+        <v>208</v>
+      </c>
+      <c r="D10" t="n">
+        <v>68</v>
+      </c>
+      <c r="E10" t="n">
+        <v>208</v>
+      </c>
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="n">
         <v>2132</v>
       </c>
-      <c r="C6">
+      <c r="C11" t="n">
         <v>600</v>
       </c>
-      <c r="D6">
+      <c r="D11" t="n">
         <v>41</v>
       </c>
-      <c r="E6">
+      <c r="E11" t="n">
         <v>89</v>
       </c>
-      <c r="F6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7">
+      <c r="F11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="n">
         <v>873</v>
       </c>
-      <c r="C7">
+      <c r="C12" t="n">
         <v>449</v>
       </c>
-      <c r="D7">
+      <c r="D12" t="n">
         <v>65</v>
       </c>
-      <c r="E7">
+      <c r="E12" t="n">
         <v>130</v>
       </c>
-      <c r="F7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8">
+      <c r="F12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="n">
         <v>3425</v>
       </c>
-      <c r="C8">
+      <c r="C13" t="n">
         <v>991</v>
       </c>
-      <c r="D8">
+      <c r="D13" t="n">
         <v>82</v>
       </c>
-      <c r="E8">
+      <c r="E13" t="n">
         <v>165</v>
       </c>
-      <c r="F8" t="s">
-        <v>19</v>
+      <c r="F13" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added final word list
</commit_message>
<xml_diff>
--- a/data/processed/progress.xlsx
+++ b/data/processed/progress.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t xml:space="preserve">language</t>
   </si>
@@ -35,64 +35,55 @@
     <t xml:space="preserve">tsum</t>
   </si>
   <si>
-    <t xml:space="preserve">82%</t>
+    <t xml:space="preserve">81%</t>
   </si>
   <si>
     <t xml:space="preserve">nubri</t>
   </si>
   <si>
-    <t xml:space="preserve">60%</t>
+    <t xml:space="preserve">59%</t>
   </si>
   <si>
     <t xml:space="preserve">nubri_namrung</t>
   </si>
   <si>
-    <t xml:space="preserve">95%</t>
-  </si>
-  <si>
     <t xml:space="preserve">nubri_lhi</t>
   </si>
   <si>
-    <t xml:space="preserve">94%</t>
-  </si>
-  <si>
     <t xml:space="preserve">nubri_lho</t>
   </si>
   <si>
     <t xml:space="preserve">nubri_sama</t>
   </si>
   <si>
-    <t xml:space="preserve">88%</t>
+    <t xml:space="preserve">76%</t>
   </si>
   <si>
     <t xml:space="preserve">nubri_sho</t>
   </si>
   <si>
-    <t xml:space="preserve">93%</t>
+    <t xml:space="preserve">80%</t>
   </si>
   <si>
     <t xml:space="preserve">gyalsumdo</t>
   </si>
   <si>
-    <t xml:space="preserve">64%</t>
+    <t xml:space="preserve">65%</t>
   </si>
   <si>
     <t xml:space="preserve">jirel</t>
   </si>
   <si>
-    <t xml:space="preserve">100%</t>
+    <t xml:space="preserve">86%</t>
   </si>
   <si>
     <t xml:space="preserve">lowa</t>
   </si>
   <si>
-    <t xml:space="preserve">43%</t>
+    <t xml:space="preserve">42%</t>
   </si>
   <si>
     <t xml:space="preserve">yolmo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">62%</t>
   </si>
   <si>
     <t xml:space="preserve">kagate</t>
@@ -464,7 +455,7 @@
         <v>81</v>
       </c>
       <c r="E2" t="n">
-        <v>171</v>
+        <v>196</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
@@ -484,7 +475,7 @@
         <v>60</v>
       </c>
       <c r="E3" t="n">
-        <v>125</v>
+        <v>144</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
@@ -504,15 +495,15 @@
         <v>68</v>
       </c>
       <c r="E4" t="n">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" t="n">
         <v>198</v>
@@ -524,15 +515,15 @@
         <v>67</v>
       </c>
       <c r="E5" t="n">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B6" t="n">
         <v>199</v>
@@ -544,15 +535,15 @@
         <v>67</v>
       </c>
       <c r="E6" t="n">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7" t="n">
         <v>185</v>
@@ -564,15 +555,15 @@
         <v>66</v>
       </c>
       <c r="E7" t="n">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B8" t="n">
         <v>195</v>
@@ -584,15 +575,15 @@
         <v>67</v>
       </c>
       <c r="E8" t="n">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B9" t="n">
         <v>2315</v>
@@ -604,15 +595,15 @@
         <v>70</v>
       </c>
       <c r="E9" t="n">
-        <v>134</v>
+        <v>158</v>
       </c>
       <c r="F9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B10" t="n">
         <v>210</v>
@@ -627,12 +618,12 @@
         <v>208</v>
       </c>
       <c r="F10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B11" t="n">
         <v>2132</v>
@@ -644,15 +635,15 @@
         <v>41</v>
       </c>
       <c r="E11" t="n">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="F11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B12" t="n">
         <v>873</v>
@@ -664,15 +655,15 @@
         <v>65</v>
       </c>
       <c r="E12" t="n">
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="F12" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B13" t="n">
         <v>3425</v>
@@ -684,10 +675,10 @@
         <v>82</v>
       </c>
       <c r="E13" t="n">
-        <v>165</v>
+        <v>193</v>
       </c>
       <c r="F13" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>